<commit_message>
Leitura dos dados do usuário e teste de enigma não-resolvido concluído
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SPREADSHEET.xlsx
+++ b/src/main/resources/DATA_SPREADSHEET.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\eclipse-workspace\desafio-phptravels\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08EB1B28-E220-431A-90FE-720BF268513A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F09CEA4-739D-4928-91F1-2FA5B4320482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1545" windowWidth="15375" windowHeight="7785" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
+    <workbookView xWindow="2550" yWindow="2235" windowWidth="15375" windowHeight="7785" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA_USER_FORM" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>NAME</t>
   </si>
@@ -50,23 +50,104 @@
     <t>COMPANY</t>
   </si>
   <si>
-    <t>Dmitr Vladmir</t>
-  </si>
-  <si>
-    <t>Marklov</t>
-  </si>
-  <si>
-    <t>automation.dvmrkolv@gmail.com</t>
-  </si>
-  <si>
-    <t>KGB</t>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Américo</t>
+  </si>
+  <si>
+    <t>Pereira</t>
+  </si>
+  <si>
+    <t>Motta</t>
+  </si>
+  <si>
+    <t>Gharib</t>
+  </si>
+  <si>
+    <t>Karim</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Zywywz</t>
+  </si>
+  <si>
+    <t>Claudiene</t>
+  </si>
+  <si>
+    <t>Wellington</t>
+  </si>
+  <si>
+    <t>Maria Rosângela</t>
+  </si>
+  <si>
+    <t>Correia de Campos</t>
+  </si>
+  <si>
+    <t>zivio.do.agape@jinnmail.comma</t>
+  </si>
+  <si>
+    <t>tonin@coldmail.froz.en</t>
+  </si>
+  <si>
+    <t>leitte_anonima@lettersweb.com</t>
+  </si>
+  <si>
+    <t>FreeSpeech multimedia</t>
+  </si>
+  <si>
+    <t>roseamerico@jinnmail.com</t>
+  </si>
+  <si>
+    <t>Mari Rosa Engenharia Civil LTDA</t>
+  </si>
+  <si>
+    <t>wbeatzz@coldmail.froz.en</t>
+  </si>
+  <si>
+    <t>FunkAgenda Produções</t>
+  </si>
+  <si>
+    <t>krmghrib_morroco@jinnmail.comma</t>
+  </si>
+  <si>
+    <t>lucas_motta_21@ibapo.ru</t>
+  </si>
+  <si>
+    <t>Ultranet DataCenters Inc.</t>
+  </si>
+  <si>
+    <t>Galeria22 Exposições e Curadoria LTDA</t>
+  </si>
+  <si>
+    <t>Restaurante Al-Bait Maghribiy LTDA</t>
+  </si>
+  <si>
+    <t>Z y Z Contabilidade S/A</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Kunrath</t>
+  </si>
+  <si>
+    <t>bruko_ultra@coldmail.froz.en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,13 +155,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,13 +207,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,49 +535,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE5699F-060C-4816-8CAE-D7528ACC6A1E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{E5AD3495-D9C2-4269-A1F2-77A8BDEE63D3}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{62C7669E-59F9-4A6E-9054-DEBB58C3F568}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{89DD2771-61A8-402C-AD0B-1AD14BFB80F5}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{30555C0C-FCEE-43B4-8DD0-2837A12793FB}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{8AD6F4C8-82A3-4558-B86A-6A64CF874548}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{D1A6F8B8-716A-4BE2-8FD6-70A0838E7E1D}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{34818A52-E558-4204-9BB5-6B5AB3557257}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{9518B607-D39C-4BE0-8AB8-B5384BC82CA3}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{44AE0353-BC93-42BF-9912-9B70B2AE7AF7}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{72F20909-F5D2-4429-AC2B-750362827ED2}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{E465F469-EE77-4EAC-B53A-C158FC5C8884}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hooks have been adjusted
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SPREADSHEET.xlsx
+++ b/src/main/resources/DATA_SPREADSHEET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\eclipse-workspace\desafio-phptravels\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F09CEA4-739D-4928-91F1-2FA5B4320482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90170131-3982-438D-88C4-29F9B1594FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2235" windowWidth="15375" windowHeight="7785" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
   </bookViews>
@@ -537,9 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE5699F-060C-4816-8CAE-D7528ACC6A1E}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Projet Fix: [1] Recovery of pom.xml; [2] Dynamism of WebDriver objects has been set; [3] Screenshot now composes a new class: EvidenceManager.java; [4] Abstract Class Steps has been set up; [5] Comments will be removed soon. After fixing, this branch must be merged directly with 'main'.
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SPREADSHEET.xlsx
+++ b/src/main/resources/DATA_SPREADSHEET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\MINI_AVALIACAO_01\mini-desafio-1-phptravel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D99977C-BD42-41E1-A327-B07057A2B7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CEC2F9-C977-47E4-9631-6953ED372C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +186,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -249,7 +241,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>

</xml_diff>

<commit_message>
Excel DSA search features: [1] Added methods to search for attribute values (ID, FIRST_NAME, LAST_NAME, EMAIL_ADDRESS, BUSINESS_NAME); [2] Needed interfaces: UserDataAttribute extending AbdstractDataAttribute; [3] DataMethods providing abstract in-common datasets methods regardless its implementation (BD, Excel, &c&al); [4] Minor fixes such as comment removal, ensuring naming conventions, Hook initializations have been made.
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SPREADSHEET.xlsx
+++ b/src/main/resources/DATA_SPREADSHEET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\MINI_AVALIACAO_01\mini-desafio-1-phptravel\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CEC2F9-C977-47E4-9631-6953ED372C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39FBEC1-03FF-4977-BB44-4A25A4772723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
   </bookViews>
@@ -131,9 +131,6 @@
     <t>bruko_ultra@coldmail.froz.en</t>
   </si>
   <si>
-    <t>INDEX</t>
-  </si>
-  <si>
     <t>Amanda</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>BUSINESS_NAME</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -559,9 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE5699F-060C-4816-8CAE-D7528ACC6A1E}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -572,19 +570,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +726,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
@@ -743,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
@@ -758,14 +756,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -774,7 +772,7 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Adding ID as a UserForm dto parameter
</commit_message>
<xml_diff>
--- a/src/main/resources/DATA_SPREADSHEET.xlsx
+++ b/src/main/resources/DATA_SPREADSHEET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\MINI_AVALIACAO_01\mini-desafio-1-phptravel\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelodeOliveiraSan\Workspace\MINI_AVALIACAO_01\mini-desafio-1-phptravels\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39FBEC1-03FF-4977-BB44-4A25A4772723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3AA95F-7F58-4651-93FF-A6D75E266298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
+    <workbookView xWindow="2895" yWindow="2580" windowWidth="15375" windowHeight="7785" xr2:uid="{24AAD396-B5F3-48AF-BC46-E6FDFDA43BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_USER_FORM" sheetId="1" r:id="rId1"/>
@@ -232,16 +232,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -557,31 +559,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AE5699F-060C-4816-8CAE-D7528ACC6A1E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="10"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -595,10 +600,10 @@
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -615,7 +620,7 @@
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -632,7 +637,7 @@
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -649,7 +654,7 @@
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -666,7 +671,7 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -683,7 +688,7 @@
       <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -700,7 +705,7 @@
       <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -722,86 +727,86 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="8">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="8">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>